<commit_message>
Updated ER-Diagram & product backlog
</commit_message>
<xml_diff>
--- a/Documents/ProductBacklog.xlsx
+++ b/Documents/ProductBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Syed\Personal\Preperation\Tennis\Working\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1AC6CB-C54E-451D-8F90-56B1DA99FD45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8051943B-C417-4BCB-A376-21AF4ADBB843}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tennis - Product Backlog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Sl No</t>
   </si>
@@ -61,13 +61,46 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Match &amp; Player API</t>
+  </si>
+  <si>
+    <t>Point, Game &amp; Set API</t>
+  </si>
+  <si>
+    <t>Business Rule Service</t>
+  </si>
+  <si>
+    <t>Persistence Service</t>
+  </si>
+  <si>
+    <t>Presentation Layer - WPF</t>
+  </si>
+  <si>
+    <t>Business logic layer to embed business rules</t>
+  </si>
+  <si>
+    <t>Persistence layer to embed database operations</t>
+  </si>
+  <si>
+    <t>View layer using WPF</t>
+  </si>
+  <si>
+    <t>Writing test cases and implemenation of API's</t>
+  </si>
+  <si>
+    <t>High level ER-Diagram</t>
+  </si>
+  <si>
+    <t>Watching tennis matches to understand the game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +108,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -92,18 +139,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,93 +623,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:H8"/>
+  <dimension ref="B3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="D5" s="2"/>
+      <c r="E5" s="8">
         <v>44485</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="12">
         <v>44486</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="19" t="s">
         <v>10</v>
       </c>
+      <c r="H5" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="D6" s="3"/>
+      <c r="E6" s="9">
         <v>44487</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="13">
+        <v>44488</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="9">
+        <v>44487</v>
+      </c>
+      <c r="F7" s="13">
+        <v>44489</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="9">
+        <v>44490</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="H8" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
-        <v>44487</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="9">
+        <v>44490</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>4</v>
-      </c>
+      <c r="H9" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="9">
+        <v>44493</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>